<commit_message>
feat: Add sample Excel file for debt management import
</commit_message>
<xml_diff>
--- a/public/file_mau_cau_hinh_cong_no.xlsx
+++ b/public/file_mau_cau_hinh_cong_no.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thachnn\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thachnn\Desktop\NKC-AutoZalo-V2\frontend\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E32C056-166E-4FB9-BDE3-88F454FE2C3C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B30F52-ECB5-46F8-8898-341E93BA2AA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{177A8859-B617-4F68-8BA8-09680CA25AAE}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>Mã Khách Hàng</t>
   </si>
@@ -300,6 +300,23 @@
   </si>
   <si>
     <t>0339562949</t>
+  </si>
+  <si>
+    <t>Mã Khách Hàng: Mã khách hàng của phiếu nợ</t>
+  </si>
+  <si>
+    <t>Loại Khách Hàng: Cố Định, Không Cố Định, Tiền Mặt</t>
+  </si>
+  <si>
+    <t>Ngày Hẹn/Lặp:
+- Cố Định: 2-7 (Tượng trưng cho từ Thứ 2 - Thứ 7)
+- Không Cố Định và Tiền Mặt: 0-10 (Tức khoảng cách giữa ngày nhắc nợ đầu tiên đến ngày nhắc nợ tiếp theo)</t>
+  </si>
+  <si>
+    <t>LƯU Ý: CÁC HEADER KHÔNG ĐƯỢC SAI SO VỚI FILE MẪU</t>
+  </si>
+  <si>
+    <t>Tên Zalo Khách Hàng: Tên zalo của khách hoặc SĐT zalo khách (Bắt buộc phải đúng)</t>
   </si>
 </sst>
 </file>
@@ -309,7 +326,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0000000000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -371,8 +388,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -389,8 +435,28 @@
         <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -465,13 +531,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -479,9 +579,23 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="5" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="3" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="6" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -506,10 +620,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
+    <cellStyle name="Bad" xfId="4" builtinId="27"/>
+    <cellStyle name="Check Cell" xfId="6" builtinId="23"/>
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
+    <cellStyle name="Input" xfId="5" builtinId="20"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="2" builtinId="10"/>
@@ -824,15 +940,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33F21070-5F8C-4EC3-8590-9C9B9A157D0E}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="74.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.140625" customWidth="1"/>
@@ -841,31 +957,31 @@
     <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <v>6</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -873,13 +989,13 @@
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <v>1</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="5" t="s">
         <v>24</v>
       </c>
     </row>
@@ -887,13 +1003,13 @@
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4">
         <v>2</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -901,13 +1017,13 @@
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
         <v>3</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -915,13 +1031,13 @@
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="4">
         <v>4</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="5" t="s">
         <v>27</v>
       </c>
     </row>
@@ -929,14 +1045,39 @@
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="6" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -959,92 +1100,92 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="10"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="18"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="6"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="14"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="6"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>